<commit_message>
Removed size constraints for notes as per gwas-template-services#69.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.8.xlsx
+++ b/schema_definitions/template_schema_v1.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC1CC0-BAF4-8542-BC84-147CD2BC7CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48A6D62-0096-984E-B0F3-DBF1C3FABA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -604,10 +604,10 @@
     <t>raw_sumstats_file</t>
   </si>
   <si>
-    <t>Raw summary stats file</t>
-  </si>
-  <si>
     <t>Raw summary statistics file</t>
+  </si>
+  <si>
+    <t>Raw summary stats file.</t>
   </si>
 </sst>
 </file>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1948,7 +1948,7 @@
         <v>187</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>24</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O22" s="6" t="b">
         <v>0</v>
@@ -4152,8 +4152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4301,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="5">
-        <v>255</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed missing size value in one of the columns
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.8.xlsx
+++ b/schema_definitions/template_schema_v1.8.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/Banking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48A6D62-0096-984E-B0F3-DBF1C3FABA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC4EE0-88DB-4248-A4AB-2EC813E43CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1992,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2651,6 +2651,9 @@
       <c r="O16" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="R16" s="12">
+        <v>-1</v>
+      </c>
     </row>
     <row r="18" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O18" s="9"/>
@@ -2667,7 +2670,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4152,7 +4155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
variant count not mandatory for curators
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.8.xlsx
+++ b/schema_definitions/template_schema_v1.8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/Banking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC4EE0-88DB-4248-A4AB-2EC813E43CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61940CFF-4D12-F248-AD5A-EBAE80AED614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -523,9 +526,6 @@
     <t>^GCST\d+$</t>
   </si>
   <si>
-    <t>readme_file</t>
-  </si>
-  <si>
     <t>Readme file</t>
   </si>
   <si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>Raw summary stats file.</t>
+  </si>
+  <si>
+    <t>readme_text</t>
   </si>
 </sst>
 </file>
@@ -1033,14 +1036,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
@@ -1073,10 +1076,10 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>152</v>
@@ -1100,16 +1103,16 @@
         <v>8</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -1230,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>26</v>
@@ -1277,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R5" s="11">
         <v>255</v>
@@ -1357,7 +1360,7 @@
         <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>35</v>
@@ -1389,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="5" t="b">
         <v>0</v>
@@ -1603,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R13" s="11">
         <v>255</v>
@@ -1688,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R15" s="11">
         <v>255</v>
@@ -1699,7 +1702,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1737,7 +1740,7 @@
         <v>158</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -1772,10 +1775,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1799,7 +1802,7 @@
         <v>24</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O18" s="9" t="b">
         <v>0</v>
@@ -1813,7 +1816,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -1846,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R19" s="11">
         <v>255</v>
@@ -1860,7 +1863,7 @@
         <v>147</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -1893,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R20" s="11">
         <v>255</v>
@@ -1904,7 +1907,7 @@
         <v>149</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1937,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R21" s="11">
         <v>255</v>
@@ -1945,10 +1948,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -1972,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O22" s="6" t="b">
         <v>0</v>
@@ -1992,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="H1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,10 +2034,10 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>152</v>
@@ -2058,16 +2061,16 @@
         <v>8</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -2213,10 +2216,10 @@
         <v>24</v>
       </c>
       <c r="J5" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="5" t="s">
@@ -2336,7 +2339,7 @@
         <v>24</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>123</v>
@@ -2377,7 +2380,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>120</v>
@@ -2708,10 +2711,10 @@
         <v>153</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>152</v>
@@ -2735,16 +2738,16 @@
         <v>8</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2814,7 +2817,7 @@
         <v>24</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>97</v>
@@ -2991,7 +2994,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="6" t="b">
         <v>1</v>
@@ -3024,10 +3027,10 @@
         <v>1</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R8" s="6">
         <v>255</v>
@@ -3147,10 +3150,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R11" s="6">
         <v>255</v>
@@ -4193,10 +4196,10 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>152</v>
@@ -4220,16 +4223,16 @@
         <v>8</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4333,7 +4336,7 @@
         <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>67</v>
@@ -4374,7 +4377,7 @@
         <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>64</v>

</xml_diff>